<commit_message>
DA 19 | Day_1_Excel
</commit_message>
<xml_diff>
--- a/Batch/18/Day_2.xlsx
+++ b/Batch/18/Day_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac217573afc2a6e8/Work/Acciojob/Modules/Excel/Batch/18/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="669" documentId="11_F25DC773A252ABDACC1048C7C19F4A1A5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85295A4C-724F-41CB-8F49-E486B1D765B1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42D25CB-FCB1-4DBA-AF00-02C13171085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
@@ -651,13 +651,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    <numFmt numFmtId="172" formatCode="dd/mmm/yyyy"/>
-    <numFmt numFmtId="173" formatCode="dd/mmmm/yyyy"/>
-    <numFmt numFmtId="174" formatCode="ddd/mmm/yyyy"/>
-    <numFmt numFmtId="175" formatCode="ddd\,\ dd/mmm/yyyy"/>
-    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="177" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="dd/mmm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mmmm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="ddd/mmm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="ddd\,\ dd/mmm/yyyy"/>
+    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -900,25 +900,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -1468,8 +1468,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>76366</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="12" name="Ink 11">
@@ -1488,7 +1488,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="12" name="Ink 11">
@@ -1533,8 +1533,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>48690</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="13" name="Ink 12">
@@ -1553,7 +1553,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="13" name="Ink 12">
@@ -1598,8 +1598,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>10681</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="24" name="Ink 23">
@@ -1618,7 +1618,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="24" name="Ink 23">
@@ -1663,8 +1663,8 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>154382</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="30" name="Ink 29">
@@ -1683,7 +1683,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="30" name="Ink 29">
@@ -1728,8 +1728,8 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>75460</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="42" name="Ink 41">
@@ -1748,7 +1748,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="42" name="Ink 41">
@@ -1793,8 +1793,8 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>940</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Ink 42">
@@ -1813,7 +1813,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Ink 42">
@@ -1858,8 +1858,8 @@
       <xdr:row>63</xdr:row>
       <xdr:rowOff>59026</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="54" name="Ink 53">
@@ -1878,7 +1878,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="54" name="Ink 53">
@@ -1923,8 +1923,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>59447</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="63" name="Ink 62">
@@ -1943,7 +1943,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="63" name="Ink 62">
@@ -1988,8 +1988,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>38648</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="64" name="Ink 63">
@@ -2008,7 +2008,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="64" name="Ink 63">
@@ -2053,8 +2053,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>556</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="69" name="Ink 68">
@@ -2073,7 +2073,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="69" name="Ink 68">
@@ -2118,8 +2118,8 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>145253</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="72" name="Ink 71">
@@ -2138,7 +2138,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="72" name="Ink 71">
@@ -2325,7 +2325,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2064.75">777 452 24575,'-15'-90'0,"14"38"0,3-90 0,1 130 0,0-1 0,1 2 0,0-1 0,0 0 0,1 1 0,1 0 0,0 0 0,1 0 0,0 1 0,0 0 0,12-12 0,-18 21 0,0-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,3 1 0,-2 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0 1 0,0 4 0,14 92 0,-5-39 0,5 112 0,-16-161 0,2 15 0,-2 0 0,-1 1 0,-11 54 0,11-75 0,0-1 0,0 0 0,0-1 0,-1 1 0,0 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0-1 0,-1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 0 0,-1 0 0,1 0 0,0-1 0,-8 3 0,9-5 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,1 0 0,-3-9 0,4 13 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,2 1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,4 5 0,42 53 0,-15-5 0,-29-45 0,1 1 0,1-2 0,0 1 0,0-1 0,1 1 0,10 9 0,-15-18 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,2-3 0,48-26 0,-11 6 0,7 5 0,-36 13 0,0 0 0,1 0 0,0 2 0,25-5 0,-28 6-1365,-1-1-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2651.34">1396 233 24575,'2'0'0,"-1"0"0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 3 0,2 11 0,-1-1 0,-1 1 0,-1 15 0,0-14 0,-12 290 0,26-14 0,-14-213 0,-1-60 0,1-1 0,1 1 0,1 0 0,1-1 0,0 1 0,1-1 0,10 32 0,2-4 0,-23-52 0,7 5 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,-2-3 0,2 0 7,0 1 0,1-1 0,-1 1 0,1 0 0,-1-1 1,1 1-1,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,2-3 0,3-3-378,0-1-1,1 1 1,18-19 0,-18 20-6455</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3618.52">1938 336 24575,'-4'9'0,"0"-1"0,0 0 0,0 0 0,-1 0 0,0 0 0,-8 8 0,-5 9 0,8-8 0,1-1 0,1 2 0,0-1 0,1 1 0,1 0 0,-6 33 0,-8 13 0,5-24 0,4 2 0,1 1 0,2 1 0,2-1 0,-1 69 0,7-104 0,1 0 0,-1 0 0,2 0 0,-1 0 0,1 0 0,0 0 0,1-1 0,0 1 0,4 8 0,-6-14 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,2-2 0,6-3 0,0 1 0,-1-2 0,0 1 0,0-2 0,-1 1 0,0-1 0,0 0 0,11-16 0,36-28 0,-48 48 0,-1 0 0,0-1 0,0 0 0,0 0 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,0-1 0,-1 1 0,1 0 0,0-10 0,-1 9 0,-2 0 0,1 0 0,-1-1 0,-1 1 0,1 0 0,-4-11 0,4 18 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,-1-1 0,2 2 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 1 0,-41 24-1365,35-23-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4660.4">1951 813 24575</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4660.39">1951 813 24575</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5218.25">2300 349 24575,'18'-3'0,"1"-1"0,-1 0 0,0-2 0,0 0 0,-1-1 0,29-16 0,21-7 0,120-59 0,-187 89-1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-10 15 201,-19 14-1685,20-24-5341</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5750.06">2376 413 24575,'-2'40'0,"1"-29"0,0 1 0,1-1 0,0 0 0,0 1 0,1-1 0,5 22 0,-5-31 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 0 0,3 1 0,63-1 0,-31-1 0,-32 1 0,0 0 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1 0 0,-1 0 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,4 5 0,-4-2 0,0-1 0,0 1 0,-1 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,-1 12 0,0-14 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1-1 0,-9 8 0,-6 5 0,-2 0 0,-29 20 0,-6 5 0,46-35 20,-1 0 0,0-1 0,0 0 0,0 0 0,-14 5 0,19-10-45,1 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-7-1 0,9 0-31,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,0-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1-2 0,-3-7-6770</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6479.21">2957 297 24575,'-1'97'0,"2"122"0,0-215 0,-1 0 0,0-1 0,1 1 0,0 0 0,-1 0 0,2-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,6 3 0,-3-3 0,-1 0 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,6-3 0,-6 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,5-8 0,33-50 0,-38 56 0,3-6 0,0 0 0,0-1 0,-2 0 0,1 0 0,-2 0 0,0 0 0,0-1 0,-1 0 0,1-18 0,-1 3 0,5-105 0,-11 214 0,-20 109 0,13-114 0,7-56 0,0 1 0,2-1 0,0 0 0,2 1 0,0-1 0,1 0 0,7 33 0,-1-39-1365</inkml:trace>
@@ -2357,7 +2357,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 491 24575,'40'0'0,"-15"1"0,0 0 0,1-2 0,-1-1 0,0-1 0,0-1 0,46-14 0,-46 10 0,-1 2 0,2 0 0,38-3 0,-10 2 0,-23 4-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="321.28">104 698 24575,'14'0'0,"-1"0"0,1-1 0,21-4 0,-30 3 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0-1 0,0 1 0,-1-1 0,1 1 0,3-6 0,29-25 0,2 2 0,82-52 0,-50 40 0,-54 35-1365,-11 5-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="321.27">104 698 24575,'14'0'0,"-1"0"0,1-1 0,21-4 0,-30 3 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0-1 0,0 1 0,-1-1 0,1 1 0,3-6 0,29-25 0,2 2 0,82-52 0,-50 40 0,-54 35-1365,-11 5-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="858.24">208 297 24575,'161'-2'0,"171"4"0,-97 23 0,-230-24 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1 0 0,-1 0 0,0 0 0,2 5 0,-3-5 0,0 0 0,-1-1 0,0 1 0,0 1 0,0-1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,-5 5 0,-7 13 0,1 0 0,-15 37 0,17-33 0,-1-2 0,-18 27 0,-58 96 0,57-93 0,28-47 0,-1 0 0,0 0 0,-1-1 0,0 0 0,0 1 0,-7 5 0,9-9 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,-1-1 0,-4 0 0,-17-1-1365,15 1-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1716.06">1304 439 24575,'0'-7'0,"-1"-12"0,1 0 0,0 0 0,2 0 0,0 0 0,1 1 0,1-1 0,1 1 0,10-28 0,-9 32 0,1 0 0,0 1 0,1-1 0,1 2 0,0-1 0,0 1 0,1 1 0,1 0 0,0 0 0,0 1 0,1 0 0,16-9 0,-6 7 0,1 0 0,42-14 0,-27 11 0,-36 14 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,3 2 0,-2-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 4 0,1 10 0,-2 1 0,1 0 0,-2 0 0,-3 29 0,-1-26 0,0-1 0,-2 1 0,-1-1 0,0 0 0,-2-1 0,0 1 0,-14 20 0,6-9 0,-18 50 0,10-37 0,21-38 0,0-1 0,0 0 0,1 1 0,0 0 0,-5 14 0,8-19 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,4 2 0,19 17 0,-18-16 0,0 1 0,0-1 0,0 1 0,-1 0 0,0 0 0,9 14 0,-13-17 0,0-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 1 0,-3 2 0,-1 1 0,0 0 0,0-1 0,-1 1 0,0-1 0,0-1 0,0 1 0,-1-1 0,0-1 0,1 1 0,-1-1 0,0 0 0,-1-1 0,1 0 0,-13 1 0,-15 2 0,0-3 0,-35-1 0,70-1 0,-10 0-273,-1 0 0,1-1 0,-1-1 0,-11-3 0,14 3-6553</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3175.57">1898 503 24575,'1'1'0,"0"-1"0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0 1 0,3 28 0,-1-16 0,-2-12 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,2 3 0,-2-5 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-2 0,4-68 0,-3 53 0,-1-32 0,0 48 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-2-2 0,2 3 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,-3 21 0,4-17 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,3 6 0,10 3-80,-15-13 85,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 1,0 0-1,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1-1-83,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 1 1,0-1 0,-1 0 0,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,-2-1 0,-4-2-6748</inkml:trace>
@@ -2454,7 +2454,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">118 0 24575,'-2'7'0,"0"-1"0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,-8 7 0,-5 7 0,10-9 0,1 0 0,0 0 0,1 0 0,-1 1 0,2 0 0,0 0 0,0 0 0,1 0 0,1 1 0,-2 15 0,0 13 0,4 69 0,2-46 0,0-48 0,1-1 0,0 0 0,1 0 0,1-1 0,0 1 0,1-1 0,12 21 0,-12-23 0,-4-8 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,6-1 0,72-4 0,-69 3 0,-5-1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,6-10 0,-1 1 0,0-1 0,-1 0 0,-1 0 0,0-1 0,11-33 0,-11 20 0,-1 0 0,-2-1 0,0 0 0,-2 0 0,-1-36 0,4 10 0,-4 48 0,0-1 0,-1 0 0,0 1 0,-1-1 0,0 0 0,0 0 0,-2-9 0,1 16 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,-3 0 0,-9-2 0,0 1 0,0 1 0,0 0 0,0 1 0,-15 2 0,22-1 0,1-1 0,-1 1 0,1 0 0,0 1 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1 1 0,-10 9 0,-72 52 0,64-53-1365,16-11-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="886.53">660 452 24575,'2'0'0,"3"0"0,3 0 0,0-2 0,-3-1 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1789.69">1163 66 24575,'-2'0'0,"-1"1"0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-3 4 0,-27 58 0,18-33 0,0-1 0,1 0 0,1 2 0,2-1 0,-9 58 0,15-62 0,2 1 0,0 0 0,5 41 0,-4-67 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,3 2 0,-1 0 0,1-1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,10 0 0,-6 0 0,0-1 0,-1 0 0,1-1 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0-1 0,1 0 0,-1 0 0,8-5 0,-1-2 0,0-1 0,0 0 0,-1-1 0,0-1 0,16-19 0,-25 25 0,0 0 0,-1 0 0,1-1 0,-1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,0 0 0,-1-1 0,0-15 0,0 7 0,-1-1 0,-1 1 0,0 0 0,-1-1 0,-1 1 0,0 0 0,-2 1 0,0-1 0,0 0 0,-11-19 0,10 23-81,5 10-18,0 1 1,-1-1-1,1 1 0,0-1 0,-1 1 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 1,-1 0-1,-2-2 0,-2 1-6727</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1789.68">1163 66 24575,'-2'0'0,"-1"1"0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-3 4 0,-27 58 0,18-33 0,0-1 0,1 0 0,1 2 0,2-1 0,-9 58 0,15-62 0,2 1 0,0 0 0,5 41 0,-4-67 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,3 2 0,-1 0 0,1-1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,10 0 0,-6 0 0,0-1 0,-1 0 0,1-1 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0-1 0,1 0 0,-1 0 0,8-5 0,-1-2 0,0-1 0,0 0 0,-1-1 0,0-1 0,16-19 0,-25 25 0,0 0 0,-1 0 0,1-1 0,-1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,0 0 0,-1-1 0,0-15 0,0 7 0,-1-1 0,-1 1 0,0 0 0,-1-1 0,-1 1 0,0 0 0,-2 1 0,0-1 0,0 0 0,-11-19 0,10 23-81,5 10-18,0 1 1,-1-1-1,1 1 0,0-1 0,-1 1 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 1,-1 0-1,-2-2 0,-2 1-6727</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2577.35">1770 156 24575,'-5'1'0,"0"0"0,0 0 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-4 5 0,-5 3 0,2 1 0,0 0 0,-10 16 0,5-3 0,0 1 0,2 0 0,-18 53 0,27-67 0,1-1 0,0 1 0,0 0 0,1 0 0,1 0 0,0 1 0,1-1 0,0 0 0,1 0 0,1 0 0,-1 1 0,5 11 0,-5-21 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,4 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0-1 0,0 1 0,0-1 0,6-4 0,-3-2 0,0-1 0,0 0 0,0 0 0,-1-1 0,-1 0 0,0 0 0,-1-1 0,0 0 0,7-20 0,-8 14 0,0 0 0,-2 0 0,3-35 0,-5 43 0,1-2 0,0-1 0,-1 1 0,-1-1 0,0 1 0,-1-1 0,0 1 0,-1 0 0,0-1 0,-1 1 0,0 0 0,-1 0 0,-6-12 0,5 16 0,-1-3 0,0 0 0,-1 1 0,0 0 0,-1 0 0,-15-14 0,21 22 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1-1 0,0 2 0,0-1 0,1 0 0,-1 0 0,0 1 0,0 0 0,0 0 0,0-1 0,0 2 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,-2 3 0,1-2-76,1 0 1,-1 0-1,1 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 1,1 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 1,0 1-1,1-1 0,-2 5 0,1 2-6750</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3145.21">2028 143 24575,'0'517'0,"0"-514"-136,0 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,0 1 0,3 4 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3924.03">2363 234 24575,'1'-2'0,"-1"0"0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 1 0,2-1 0,42-9 0,-35 9 0,4 0 0,-1 1 0,1 0 0,0 0 0,24 5 0,-35-4 0,0 1 0,-1-1 0,1 0 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 1 0,0 0 0,2 5 0,2 17 0,-1-1 0,0 1 0,-2 0 0,-1 1 0,-2-1 0,0 0 0,-6 39 0,4-49 0,-2 0 0,0 0 0,-1 0 0,0-1 0,-1 0 0,-1 0 0,-1-1 0,-9 16 0,-23 49 0,12-28 0,21-40 0,0 1 0,1 0 0,-5 15 0,10-26 0,1 0 0,-1 0 0,0 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,1-3 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,2-2 0,23-19 0,1 0 0,1 1 0,44-25 0,85-56 0,-157 103-23,2-1-38,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1-3 0,0-1-6765</inkml:trace>
@@ -2519,7 +2519,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 312 24575,'13'103'0,"-15"1"0,4 115 0,-2-216 0,0-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,2 2 0,9 11 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="615.92">413 506 24575,'0'7'0,"3"35"0,-3-41 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,2 0 0,-1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1-2 0,2-44 0,-10 30-1365,3 12-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="615.91">413 506 24575,'0'7'0,"3"35"0,-3-41 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,2 0 0,-1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1-2 0,2-44 0,-10 30-1365,3 12-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1683.4">839 441 24575,'-12'-45'0,"1"10"0,10 27 0,-1-1 0,2 1 0,-1-1 0,1 0 0,0 1 0,1-1 0,0 1 0,1-1 0,-1 1 0,2 0 0,-1-1 0,1 1 0,0 0 0,1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,11-11 0,-6 7 0,1 1 0,0 1 0,0 0 0,1 0 0,0 1 0,0 0 0,1 1 0,0 1 0,16-7 0,-18 10 0,0 0 0,0 1 0,0 0 0,19-1 0,2 0 0,-28 3 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 4 0,4 8 0,0 1 0,-2 0 0,4 28 0,-4-17 0,1-2 0,-2 1 0,0-1 0,-2 1 0,0-1 0,-2 0 0,-1 1 0,-1-1 0,-1 0 0,-1-1 0,-1 1 0,-15 34 0,16-47 0,-1 0 0,1-1 0,-2 0 0,1 0 0,-2 0 0,1-1 0,-17 14 0,-73 49 0,48-51 0,24-20 0,25-2 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,3 0 0,57-1 0,-51 1 0,3 1 0,1 0 0,-1 0 0,0 2 0,0-1 0,0 2 0,0 0 0,-1 1 0,0 0 0,25 14 0,-38-19-21,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-7 1-6804</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2521.67">1420 221 24575,'0'-9'0,"4"-80"0,-4 81 0,2-1 0,-1 1 0,1-1 0,0 1 0,1-1 0,0 1 0,8-14 0,-9 18 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,7-3 0,-9 4 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,1 2 0,5 15 0,-1 1 0,-2 0 0,0 0 0,0 0 0,-1 24 0,3 8 0,-4-39 0,0-1 0,-1 0 0,0 1 0,-1-1 0,0 1 0,-1-1 0,0 1 0,-1-1 0,0 0 0,-1 0 0,-1 0 0,-8 19 0,-38 82 0,55-109 0,1-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,10 3 0,25 2 0,-35-6 0,1-1 0,-1 1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 1 0,0 0 0,7 5 0,22 11 0,-26-15 0,0 0 0,-1 1 0,0-1 0,0 2 0,0-1 0,9 9 0,-16-13 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 2 0,0 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-5 3 0,-4 2 0,0 0 0,0-1 0,-1-1 0,0 0 0,-13 3 0,11-4 0,1 1 0,0 1 0,0 0 0,-13 7 0,4-1-68,18-10-13,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1 0-1,1 0 1,0 0 0,0 0 0,1 1 0,-4 4 0</inkml:trace>
 </inkml:ink>
@@ -2845,7 +2845,7 @@
   <dimension ref="A2:B14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2960,7 +2960,7 @@
       <c r="B8" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>123456</v>
       </c>
     </row>
@@ -2968,7 +2968,7 @@
       <c r="B9" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>123456</v>
       </c>
     </row>
@@ -2984,7 +2984,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>123456</v>
       </c>
       <c r="D11" t="s">
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <v>123456</v>
       </c>
       <c r="D12" t="s">
@@ -3000,7 +3000,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <v>123456</v>
       </c>
       <c r="D13" t="s">
@@ -3008,7 +3008,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>123456</v>
       </c>
       <c r="D14" t="s">
@@ -3019,7 +3019,7 @@
       <c r="B15" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="29">
         <v>123456</v>
       </c>
     </row>
@@ -3052,7 +3052,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="30">
         <v>0</v>
       </c>
     </row>
@@ -3066,7 +3066,7 @@
       <c r="G21">
         <v>3</v>
       </c>
-      <c r="I21" s="31">
+      <c r="I21" s="30">
         <v>0.125</v>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       <c r="H22">
         <v>0.25</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="30">
         <v>0.25</v>
       </c>
     </row>
@@ -3085,7 +3085,7 @@
       <c r="G23">
         <v>9</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="30">
         <v>0.375</v>
       </c>
     </row>
@@ -3096,7 +3096,7 @@
       <c r="H24">
         <v>0.5</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="30">
         <v>0.5</v>
       </c>
     </row>
@@ -3104,7 +3104,7 @@
       <c r="G25">
         <v>15</v>
       </c>
-      <c r="I25" s="31">
+      <c r="I25" s="30">
         <v>0.625</v>
       </c>
     </row>
@@ -3115,7 +3115,7 @@
       <c r="H26">
         <v>0.75</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="30">
         <v>0.75</v>
       </c>
     </row>
@@ -3123,7 +3123,7 @@
       <c r="G27">
         <v>21</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="30">
         <v>0.875</v>
       </c>
     </row>
@@ -3134,7 +3134,7 @@
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="30">
         <v>1</v>
       </c>
     </row>
@@ -3168,10 +3168,10 @@
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <v>0</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="31">
         <v>1</v>
       </c>
     </row>
@@ -3179,51 +3179,51 @@
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E40" s="33"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D41">
         <v>0.25</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E42" s="33"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D43">
         <v>0.5</v>
       </c>
-      <c r="E43" s="33">
+      <c r="E43" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E44" s="33"/>
+      <c r="E44" s="32"/>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D45">
         <v>0.75</v>
       </c>
-      <c r="E45" s="33">
+      <c r="E45" s="32">
         <v>0.75</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="E46" s="33"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="33">
+      <c r="E47" s="32">
         <v>1</v>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.45">
-      <c r="D61" s="34">
+      <c r="D61" s="33">
         <v>1.2340000000000001E-3</v>
       </c>
     </row>
@@ -3258,7 +3258,7 @@
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.45">
-      <c r="F71" s="35" t="s">
+      <c r="F71" s="34" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3273,8 +3273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8461831-83C1-4205-9F0E-51061F62C823}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3450,8 +3450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE94A817-FE9D-4137-85BB-57309350B450}">
   <dimension ref="B2:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3518,7 +3518,7 @@
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="1">
         <f ca="1">TODAY()</f>
-        <v>45774</v>
+        <v>45816</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -3712,8 +3712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D037B940-882F-4AEC-B5F6-5C8FCB360459}">
   <dimension ref="B2:K79"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4789,43 +4789,43 @@
     </row>
     <row r="26" spans="2:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
     <row r="29" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C36" s="20"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C38" s="21"/>
+      <c r="C38" s="20"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C40" s="22"/>
+      <c r="C40" s="21"/>
     </row>
     <row r="43" spans="3:5" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="22" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>